<commit_message>
proj_results_reporting: fix some small formatting issues in the data definition file.
</commit_message>
<xml_diff>
--- a/public/attachments/proj_results_reporting_data_defs.xlsx
+++ b/public/attachments/proj_results_reporting_data_defs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tibbs001/work/aact-proj-1/public/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF082F5D-C4A2-CA4B-8307-220F78F7F2A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC76E591-3258-5246-8252-174BB7E4728E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="460" windowWidth="25300" windowHeight="11180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="460" windowWidth="25300" windowHeight="11180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Definitions" sheetId="3" r:id="rId1"/>
@@ -29,24 +29,12 @@
     <t>url</t>
   </si>
   <si>
-    <t>NCT_ID</t>
-  </si>
-  <si>
     <t>verification_year</t>
   </si>
   <si>
     <t>verification_month</t>
   </si>
   <si>
-    <t>BRIEF_TITLE</t>
-  </si>
-  <si>
-    <t>NUMBER_OF_ARMS</t>
-  </si>
-  <si>
-    <t>ENROLLMENT</t>
-  </si>
-  <si>
     <t>start_month</t>
   </si>
   <si>
@@ -168,9 +156,6 @@
   </si>
   <si>
     <t>delayed12</t>
-  </si>
-  <si>
-    <t>RESPONSIBLE_PARTY_TYPE</t>
   </si>
   <si>
     <t>sponsor_name</t>
@@ -479,6 +464,21 @@
   <si>
     <t>Sponsors and Funding</t>
     <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>enrollment</t>
+  </si>
+  <si>
+    <t>number_of_arms</t>
+  </si>
+  <si>
+    <t>brief_title</t>
+  </si>
+  <si>
+    <t>nct_id</t>
+  </si>
+  <si>
+    <t>responsible_party_type</t>
   </si>
 </sst>
 </file>
@@ -824,7 +824,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -939,58 +939,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1036,28 +984,27 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1381,865 +1328,866 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8CADDE-082A-7148-92DE-02B6F30D42A4}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" customWidth="1"/>
-    <col min="3" max="4" width="52.33203125" customWidth="1"/>
-    <col min="5" max="5" width="65.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="52.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="65.1640625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>146</v>
+    <row r="1" spans="1:5" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>147</v>
+      <c r="A2" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>147</v>
+      <c r="A3" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="D8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="D10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>147</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="C23" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>147</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>147</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>147</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>147</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>147</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>147</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>147</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>147</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>147</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>147</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>147</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>147</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>147</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>147</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E21" s="3" t="s">
+      <c r="C27" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>147</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>147</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>147</v>
-      </c>
-      <c r="B24" s="2" t="s">
+    </row>
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>147</v>
-      </c>
-      <c r="B25" s="6" t="s">
+      <c r="C29" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>147</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>147</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>147</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>147</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>147</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="D30" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>147</v>
+      <c r="A31" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>147</v>
+      <c r="A32" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>147</v>
+      <c r="A33" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
     <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>147</v>
+      <c r="A34" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>147</v>
+      <c r="A35" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>147</v>
+      <c r="A36" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>147</v>
+      <c r="A37" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>147</v>
+      <c r="A38" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>147</v>
+      <c r="A39" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>147</v>
+      <c r="A40" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>147</v>
+      <c r="A41" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>147</v>
+      <c r="A42" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>147</v>
+      <c r="A43" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>147</v>
-      </c>
-      <c r="B44" s="2" t="s">
+      <c r="D47" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E44" s="3"/>
-    </row>
-    <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>147</v>
-      </c>
-      <c r="B45" s="2" t="s">
+      <c r="C50" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E45" s="3"/>
-    </row>
-    <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>147</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E46" s="3"/>
-    </row>
-    <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>147</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E47" s="3"/>
-    </row>
-    <row r="48" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>147</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>147</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E49" s="3" t="s">
+      <c r="C53" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>147</v>
-      </c>
-      <c r="B50" s="2" t="s">
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="112" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>147</v>
-      </c>
-      <c r="B51" s="2" t="s">
+      <c r="C54" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>147</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C52" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E52" s="3" t="s">
+      <c r="D55" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>147</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E53" s="3"/>
-    </row>
-    <row r="54" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>147</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="96" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>147</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2255,7 +2203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B879A9A-B3D8-EF4E-882E-2B64D6538058}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -2268,42 +2216,42 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>

</xml_diff>

<commit_message>
small changes to Results Reporting Data Defs
</commit_message>
<xml_diff>
--- a/public/attachments/proj_results_reporting_data_defs.xlsx
+++ b/public/attachments/proj_results_reporting_data_defs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tibbs001/work/aact-proj-1/public/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC76E591-3258-5246-8252-174BB7E4728E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BA6FA3-A09B-B24B-B1AD-8ABA70EF8815}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="460" windowWidth="25300" windowHeight="11180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,12 @@
     <sheet name="Data Definitions" sheetId="3" r:id="rId1"/>
     <sheet name="General Info" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="148">
   <si>
     <t>responsible_party_organization</t>
   </si>
@@ -455,14 +455,6 @@
   </si>
   <si>
     <t>analyzed_studies</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Study Design Characteristics</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sponsors and Funding</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
@@ -485,7 +477,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -616,15 +608,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -984,7 +967,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -993,15 +976,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1326,10 +1303,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8CADDE-082A-7148-92DE-02B6F30D42A4}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1341,20 +1318,20 @@
     <col min="6" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1363,7 +1340,7 @@
         <v>142</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>54</v>
@@ -1393,7 +1370,7 @@
         <v>142</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>56</v>
@@ -1604,92 +1581,96 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="B18" s="5" t="s">
+    <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="C18" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>146</v>
+        <v>18</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>73</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>73</v>
@@ -1701,57 +1682,63 @@
         <v>142</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>83</v>
       </c>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>83</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1759,78 +1746,74 @@
         <v>142</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>46</v>
+        <v>147</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>83</v>
       </c>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>83</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>149</v>
+        <v>30</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1838,27 +1821,29 @@
         <v>142</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
+      <c r="E33" s="3" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1866,14 +1851,14 @@
         <v>142</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1881,14 +1866,14 @@
         <v>142</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1896,14 +1881,14 @@
         <v>142</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1911,14 +1896,14 @@
         <v>142</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1926,14 +1911,14 @@
         <v>142</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1941,29 +1926,29 @@
         <v>142</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1971,40 +1956,40 @@
         <v>142</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3" t="s">
-        <v>115</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E43" s="3"/>
     </row>
     <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>116</v>
@@ -2016,185 +2001,151 @@
         <v>142</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>116</v>
       </c>
       <c r="E45" s="3"/>
     </row>
-    <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E46" s="3"/>
-    </row>
-    <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="E46" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E47" s="3"/>
+      <c r="E47" s="3" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="48" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>116</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>116</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>129</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="E53" s="3"/>
-    </row>
-    <row r="54" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="96" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E55" s="3" t="s">
+      <c r="E53" s="3" t="s">
         <v>136</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B25:E25"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>